<commit_message>
(#230) corrected test data
</commit_message>
<xml_diff>
--- a/test-data/cts_advanced_search_cancer_type_data.xlsx
+++ b/test-data/cts_advanced_search_cancer_type_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681DC59C-D50E-43DD-A4B8-E8B4277F9B3C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5768F13-921C-264B-A41D-273E5D6EC445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="6380" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cancertype" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>path</t>
   </si>
@@ -138,9 +138,6 @@
     <t>fin=C115197&amp;loc=0&amp;rl=2&amp;st=C160920&amp;t=C487</t>
   </si>
   <si>
-    <t>fin=C115197&amp;loc=0&amp;rl=2&amp;st=C160920&amp;t=C4872</t>
-  </si>
-  <si>
     <t>Astra</t>
   </si>
   <si>
@@ -184,6 +181,12 @@
   </si>
   <si>
     <t>loc=0&amp;rl=2&amp;st=C7489&amp;stg=C7794&amp;t=C9291</t>
+  </si>
+  <si>
+    <t>fin=C28306&amp;loc=0&amp;rl=2&amp;t=C9291</t>
+  </si>
+  <si>
+    <t>fin=C115197&amp;loc=0&amp;rl=2&amp;stg=C94774&amp;t=C4872</t>
   </si>
 </sst>
 </file>
@@ -547,25 +550,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="5" width="19.36328125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="24" style="4" customWidth="1"/>
-    <col min="8" max="8" width="25.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="25.90625" style="4" customWidth="1"/>
-    <col min="11" max="12" width="32.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.7265625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="47.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="43.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="56" style="4" customWidth="1"/>
+    <col min="10" max="10" width="46" style="4" customWidth="1"/>
+    <col min="11" max="11" width="47.1640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="45.6640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="38.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -647,7 +653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -682,51 +688,51 @@
         <v>37</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -744,15 +750,15 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.54296875" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.453125" customWidth="1"/>
+    <col min="1" max="1" width="51.5" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,7 +766,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -768,12 +774,12 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -798,15 +804,15 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -823,12 +829,12 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -836,16 +842,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="H2" s="4"/>
     </row>

</xml_diff>